<commit_message>
add shorting nb; edit repos
</commit_message>
<xml_diff>
--- a/excel/10_leverage.xlsx
+++ b/excel/10_leverage.xlsx
@@ -8,13 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\busi448\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C45CDD8-B232-48F6-83F3-A0815FBE5235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1A7180-2633-45CD-873B-BB9832FC5EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14490" yWindow="9980" windowWidth="9380" windowHeight="6410" xr2:uid="{85997A6B-105C-45C3-9CB4-DBADA1C8AA17}"/>
+    <workbookView xWindow="33700" yWindow="3120" windowWidth="9380" windowHeight="6410" xr2:uid="{85997A6B-105C-45C3-9CB4-DBADA1C8AA17}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Margin" sheetId="1" r:id="rId1"/>
+    <sheet name="Repo" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="haircut">Repo!$E$2</definedName>
+    <definedName name="init_cash">Repo!$C$3</definedName>
+    <definedName name="leverage">Repo!$C$13</definedName>
+    <definedName name="MV">Repo!$C$2</definedName>
+    <definedName name="repo_price">Repo!$C$4</definedName>
+    <definedName name="repo_rate">Repo!$E$3</definedName>
+    <definedName name="return">Repo!$C$17</definedName>
+    <definedName name="term">Repo!$C$5</definedName>
+  </definedNames>
   <calcPr calcId="191029" iterate="1" iterateCount="1000"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>Assets</t>
   </si>
@@ -61,6 +72,54 @@
   </si>
   <si>
     <t>Balance Sheet after Realized Return (ignoring interest exp)</t>
+  </si>
+  <si>
+    <t>Assumptions</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>Implied haircut</t>
+  </si>
+  <si>
+    <t>Initial cash</t>
+  </si>
+  <si>
+    <t>Implied repo rate</t>
+  </si>
+  <si>
+    <t>Repurchase price</t>
+  </si>
+  <si>
+    <t>Term (days)</t>
+  </si>
+  <si>
+    <t>Initial Balance Sheet (buy bond and borrow in repo market)</t>
+  </si>
+  <si>
+    <t>Bond (repo'd)</t>
+  </si>
+  <si>
+    <t>Repo (Cash Loan)</t>
+  </si>
+  <si>
+    <t>Leverage</t>
+  </si>
+  <si>
+    <t>Percent margin</t>
+  </si>
+  <si>
+    <t>Balance Sheet after Realized Return (prior to returning cash)</t>
+  </si>
+  <si>
+    <t>Bond return (total)</t>
+  </si>
+  <si>
+    <t>Levered return</t>
+  </si>
+  <si>
+    <t>Levered return (formula)</t>
   </si>
 </sst>
 </file>
@@ -70,7 +129,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -288,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -320,13 +379,29 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -644,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2257A83-6B46-4E2D-883C-BCBE65BA1E2C}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -795,4 +870,305 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8774C3A8-E238-4BA2-A94C-E40054297607}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.36328125" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="10.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="20">
+        <v>1000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="12">
+        <f>1-init_cash/MV</f>
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="F2" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(haircut)</f>
+        <v>=1-init_cash/MV</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="20">
+        <v>980</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="12">
+        <f>(repo_price/init_cash-1)*360/term</f>
+        <v>3.6734693877547464E-2</v>
+      </c>
+      <c r="F3" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(repo_rate)</f>
+        <v>=(repo_price/init_cash-1)*360/term</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="20">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="13">
+        <f>MV</f>
+        <v>1000</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="16">
+        <f>init_cash</f>
+        <v>980</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="5"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="17">
+        <f>C11-E9</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="6"/>
+      <c r="C11" s="15">
+        <f>SUM(C9:C10)</f>
+        <v>1000</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="18">
+        <f>SUM(E9:E10)</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="21"/>
+      <c r="C12" s="13"/>
+      <c r="E12" s="22"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="24">
+        <f>E9/E10</f>
+        <v>49</v>
+      </c>
+      <c r="D13" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(C13)</f>
+        <v>=E9/E10</v>
+      </c>
+      <c r="E13" s="22"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="12">
+        <f>E10/C11</f>
+        <v>0.02</v>
+      </c>
+      <c r="D14" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(C14)</f>
+        <v>=E10/C11</v>
+      </c>
+      <c r="E14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="21"/>
+      <c r="C15" s="13"/>
+      <c r="E15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="1"/>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="25">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="11"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="13">
+        <f>C9*(1+return)</f>
+        <v>1004.9999999999999</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="16">
+        <f>repo_price</f>
+        <v>981</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B20" s="5"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="17">
+        <f>C21-E19</f>
+        <v>23.999999999999886</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="6"/>
+      <c r="C21" s="15">
+        <f>SUM(C19:C20)</f>
+        <v>1004.9999999999999</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="18">
+        <f>SUM(E19:E20)</f>
+        <v>1004.9999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="21"/>
+      <c r="C22" s="13"/>
+      <c r="E22" s="22"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="24">
+        <f>E19/E20</f>
+        <v>40.875000000000192</v>
+      </c>
+      <c r="D23" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(C23)</f>
+        <v>=E19/E20</v>
+      </c>
+      <c r="E23" s="22"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B24" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="12">
+        <f>E20/C21</f>
+        <v>2.3880597014925262E-2</v>
+      </c>
+      <c r="D24" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(C24)</f>
+        <v>=E20/C21</v>
+      </c>
+      <c r="E24" s="22"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B25" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="12">
+        <f>E20/E10-1</f>
+        <v>0.1999999999999944</v>
+      </c>
+      <c r="D25" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(C25)</f>
+        <v>=E20/E10-1</v>
+      </c>
+      <c r="E25" s="22"/>
+    </row>
+    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B26" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="27">
+        <f>return+leverage*(return-repo_rate*term/360)</f>
+        <v>0.20000000000000484</v>
+      </c>
+      <c r="D26" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(C26)</f>
+        <v>=return+leverage*(return-repo_rate*term/360)</v>
+      </c>
+      <c r="E26" s="22"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="23"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>